<commit_message>
add org to import
</commit_message>
<xml_diff>
--- a/storage/app/AE Marker - Project Import Template.xlsx
+++ b/storage/app/AE Marker - Project Import Template.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/aec-portfolio/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49B69693-6C23-A446-9652-E46556985C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C677C1-B6E3-A44B-9467-C4715B85992D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38980" yWindow="-21480" windowWidth="27240" windowHeight="16440" xr2:uid="{21569DC4-0C9C-9A4F-A7E1-7EA7911B1920}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>budget_usd</t>
+  </si>
+  <si>
+    <t>organisation</t>
   </si>
 </sst>
 </file>
@@ -411,22 +414,28 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove org from excel template
</commit_message>
<xml_diff>
--- a/storage/app/AE Marker - Project Import Template.xlsx
+++ b/storage/app/AE Marker - Project Import Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/aec-portfolio/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C677C1-B6E3-A44B-9467-C4715B85992D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192760BB-A3DE-914B-8520-C08C587B3262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38980" yWindow="-21480" windowWidth="27240" windowHeight="16440" xr2:uid="{21569DC4-0C9C-9A4F-A7E1-7EA7911B1920}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>name</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>budget_usd</t>
-  </si>
-  <si>
-    <t>organisation</t>
   </si>
 </sst>
 </file>
@@ -411,31 +408,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D307094-3E81-F641-AFEE-64FC4819F8D6}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add countries but not to import: - add start and end dates also to import
</commit_message>
<xml_diff>
--- a/storage/app/AE Marker - Project Import Template.xlsx
+++ b/storage/app/AE Marker - Project Import Template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/aec-portfolio/storage/app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/aec_portfolio/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192760BB-A3DE-914B-8520-C08C587B3262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63DB854-5F29-7A4C-BA96-5D7BF6D13A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38980" yWindow="-21480" windowWidth="27240" windowHeight="16440" xr2:uid="{21569DC4-0C9C-9A4F-A7E1-7EA7911B1920}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{21569DC4-0C9C-9A4F-A7E1-7EA7911B1920}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="projects" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -47,14 +47,44 @@
     <t>description</t>
   </si>
   <si>
-    <t>budget_usd</t>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>enter a unique code for the project</t>
+  </si>
+  <si>
+    <t>the project name</t>
+  </si>
+  <si>
+    <t>the project description</t>
+  </si>
+  <si>
+    <t>the budget for the project</t>
+  </si>
+  <si>
+    <t>the 3-letter code for the currency (e.g. USD or EUR)</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>the start date of the project (can be left blank)</t>
+  </si>
+  <si>
+    <t>the end date of the project (can be left blank)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,6 +96,20 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,9 +135,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,15 +456,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D307094-3E81-F641-AFEE-64FC4819F8D6}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -427,8 +482,45 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="37" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
handle dates in import
</commit_message>
<xml_diff>
--- a/storage/app/AE Marker - Project Import Template.xlsx
+++ b/storage/app/AE Marker - Project Import Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/aec_portfolio/storage/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63DB854-5F29-7A4C-BA96-5D7BF6D13A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D62B1BA-CB6A-074C-9751-6A2782DB34AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{21569DC4-0C9C-9A4F-A7E1-7EA7911B1920}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -78,13 +78,25 @@
   </si>
   <si>
     <t>the end date of the project (can be left blank)</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Project name</t>
+  </si>
+  <si>
+    <t>description of the project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -114,13 +126,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,13 +166,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,17 +498,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D307094-3E81-F641-AFEE-64FC4819F8D6}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="14" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="6" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
   </cols>
@@ -487,10 +532,10 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="1"/>
@@ -498,31 +543,62 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="37" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="9">
+        <v>500000</v>
+      </c>
+      <c r="F3" s="10">
+        <v>44896</v>
+      </c>
+      <c r="G3" s="10">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F5" s="4"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>